<commit_message>
new experiments c8 script and adjustments for enabling 0action boosting
</commit_message>
<xml_diff>
--- a/num_updats_calculations.xlsx
+++ b/num_updats_calculations.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="6">
   <si>
     <t>num_updates</t>
   </si>
@@ -40,12 +40,15 @@
   <si>
     <t>Bemerkung</t>
   </si>
+  <si>
+    <t>updates per year</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -53,16 +56,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -70,14 +86,32 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Berechnung" xfId="1" builtinId="22"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -356,15 +390,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -374,14 +408,32 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K1" t="s">
+        <v>4</v>
+      </c>
+      <c r="M1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>500</v>
       </c>
@@ -391,12 +443,29 @@
       <c r="C2">
         <v>8</v>
       </c>
-      <c r="D2">
-        <f>A2*B2*C2</f>
+      <c r="D2" s="1">
+        <f t="shared" ref="D2:D10" si="0">A2*B2*C2</f>
         <v>1456000</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G2">
+        <v>2912000</v>
+      </c>
+      <c r="H2">
+        <v>14</v>
+      </c>
+      <c r="I2">
+        <v>15</v>
+      </c>
+      <c r="J2" s="1">
+        <f>G2/H2/I2</f>
+        <v>13866.666666666666</v>
+      </c>
+      <c r="M2">
+        <f>364/H2</f>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>500</v>
       </c>
@@ -407,12 +476,12 @@
       <c r="C3">
         <v>8</v>
       </c>
-      <c r="D3">
-        <f>A3*B3*C3</f>
+      <c r="D3" s="1">
+        <f t="shared" si="0"/>
         <v>2912000</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>500</v>
       </c>
@@ -423,12 +492,12 @@
       <c r="C4">
         <v>8</v>
       </c>
-      <c r="D4">
-        <f>A4*B4*C4</f>
+      <c r="D4" s="1">
+        <f t="shared" si="0"/>
         <v>4368000</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1000</v>
       </c>
@@ -438,12 +507,12 @@
       <c r="C5">
         <v>8</v>
       </c>
-      <c r="D5">
-        <f>A5*B5*C5</f>
+      <c r="D5" s="1">
+        <f t="shared" si="0"/>
         <v>1456000</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1000</v>
       </c>
@@ -453,12 +522,12 @@
       <c r="C6">
         <v>8</v>
       </c>
-      <c r="D6">
-        <f>A6*B6*C6</f>
+      <c r="D6" s="1">
+        <f t="shared" si="0"/>
         <v>2912000</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1000</v>
       </c>
@@ -469,12 +538,12 @@
       <c r="C7">
         <v>8</v>
       </c>
-      <c r="D7">
-        <f>A7*B7*C7</f>
+      <c r="D7" s="1">
+        <f t="shared" si="0"/>
         <v>5824000</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1000</v>
       </c>
@@ -485,12 +554,12 @@
       <c r="C8">
         <v>8</v>
       </c>
-      <c r="D8">
-        <f>A8*B8*C8</f>
+      <c r="D8" s="1">
+        <f t="shared" si="0"/>
         <v>8736000</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2000</v>
       </c>
@@ -501,9 +570,24 @@
       <c r="C9">
         <v>8</v>
       </c>
-      <c r="D9">
-        <f>A9*B9*C9</f>
+      <c r="D9" s="1">
+        <f t="shared" si="0"/>
         <v>2912000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>10000</v>
+      </c>
+      <c r="B10">
+        <v>14</v>
+      </c>
+      <c r="C10">
+        <v>15</v>
+      </c>
+      <c r="D10" s="1">
+        <f t="shared" si="0"/>
+        <v>2100000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
dummy file for feudal algo. ray_main for using ray for parallelleization
</commit_message>
<xml_diff>
--- a/num_updats_calculations.xlsx
+++ b/num_updats_calculations.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="7">
   <si>
     <t>num_updates</t>
   </si>
@@ -42,6 +42,9 @@
   </si>
   <si>
     <t>updates per year</t>
+  </si>
+  <si>
+    <t>c8</t>
   </si>
 </sst>
 </file>
@@ -78,7 +81,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -101,14 +104,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Berechnung" xfId="1" builtinId="22"/>
@@ -390,10 +405,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M10"/>
+  <dimension ref="A1:M12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -429,7 +444,7 @@
       <c r="K1" t="s">
         <v>4</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
@@ -444,7 +459,7 @@
         <v>8</v>
       </c>
       <c r="D2" s="1">
-        <f t="shared" ref="D2:D10" si="0">A2*B2*C2</f>
+        <f t="shared" ref="D2:D11" si="0">A2*B2*C2</f>
         <v>1456000</v>
       </c>
       <c r="G2">
@@ -460,7 +475,7 @@
         <f>G2/H2/I2</f>
         <v>13866.666666666666</v>
       </c>
-      <c r="M2">
+      <c r="M2" s="1">
         <f>364/H2</f>
         <v>26</v>
       </c>
@@ -480,6 +495,26 @@
         <f t="shared" si="0"/>
         <v>2912000</v>
       </c>
+      <c r="G3">
+        <v>2912000</v>
+      </c>
+      <c r="H3">
+        <v>14</v>
+      </c>
+      <c r="I3">
+        <v>10</v>
+      </c>
+      <c r="J3" s="1">
+        <f>G3/H3/I3</f>
+        <v>20800</v>
+      </c>
+      <c r="K3" t="s">
+        <v>6</v>
+      </c>
+      <c r="M3" s="1">
+        <f>364/H3</f>
+        <v>26</v>
+      </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4">
@@ -588,6 +623,36 @@
       <c r="D10" s="1">
         <f t="shared" si="0"/>
         <v>2100000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>20000</v>
+      </c>
+      <c r="B11">
+        <v>14</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11" s="2">
+        <f t="shared" si="0"/>
+        <v>280000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>100000</v>
+      </c>
+      <c r="B12">
+        <v>14</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12" s="2">
+        <f t="shared" ref="D12" si="1">A12*B12*C12</f>
+        <v>1400000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ray version for c9 config
</commit_message>
<xml_diff>
--- a/num_updats_calculations.xlsx
+++ b/num_updats_calculations.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="9">
   <si>
     <t>num_updates</t>
   </si>
@@ -45,6 +45,12 @@
   </si>
   <si>
     <t>c8</t>
+  </si>
+  <si>
+    <t>c9</t>
+  </si>
+  <si>
+    <t>number of years simulated</t>
   </si>
 </sst>
 </file>
@@ -405,15 +411,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M12"/>
+  <dimension ref="A1:O13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -447,8 +453,11 @@
       <c r="M1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>500</v>
       </c>
@@ -479,8 +488,12 @@
         <f>364/H2</f>
         <v>26</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O2" s="1">
+        <f>J2/M2</f>
+        <v>533.33333333333326</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>500</v>
       </c>
@@ -515,8 +528,12 @@
         <f>364/H3</f>
         <v>26</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="O3" s="1">
+        <f t="shared" ref="O3:O6" si="1">J3/M3</f>
+        <v>800</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>500</v>
       </c>
@@ -531,8 +548,29 @@
         <f t="shared" si="0"/>
         <v>4368000</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="G4">
+        <v>2912000</v>
+      </c>
+      <c r="H4">
+        <v>14</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4" s="1">
+        <f>G4/H4/I4</f>
+        <v>208000</v>
+      </c>
+      <c r="M4" s="1">
+        <f>364/H4</f>
+        <v>26</v>
+      </c>
+      <c r="O4" s="1">
+        <f t="shared" si="1"/>
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1000</v>
       </c>
@@ -546,8 +584,29 @@
         <f t="shared" si="0"/>
         <v>1456000</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="G5">
+        <v>1400000</v>
+      </c>
+      <c r="H5">
+        <v>14</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="J5" s="1">
+        <f>G5/H5/I5</f>
+        <v>100000</v>
+      </c>
+      <c r="M5" s="1">
+        <f>364/H5</f>
+        <v>26</v>
+      </c>
+      <c r="O5" s="1">
+        <f t="shared" si="1"/>
+        <v>3846.1538461538462</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1000</v>
       </c>
@@ -561,8 +620,32 @@
         <f t="shared" si="0"/>
         <v>2912000</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="G6">
+        <v>1456000</v>
+      </c>
+      <c r="H6">
+        <v>14</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6" s="2">
+        <f>G6/H6/I6</f>
+        <v>104000</v>
+      </c>
+      <c r="K6" t="s">
+        <v>7</v>
+      </c>
+      <c r="M6" s="2">
+        <f>364/H6</f>
+        <v>26</v>
+      </c>
+      <c r="O6" s="2">
+        <f t="shared" si="1"/>
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1000</v>
       </c>
@@ -578,7 +661,7 @@
         <v>5824000</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1000</v>
       </c>
@@ -594,7 +677,7 @@
         <v>8736000</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2000</v>
       </c>
@@ -610,7 +693,7 @@
         <v>2912000</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>10000</v>
       </c>
@@ -625,7 +708,7 @@
         <v>2100000</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>20000</v>
       </c>
@@ -635,12 +718,12 @@
       <c r="C11">
         <v>1</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11" s="1">
         <f t="shared" si="0"/>
         <v>280000</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>100000</v>
       </c>
@@ -650,9 +733,24 @@
       <c r="C12">
         <v>1</v>
       </c>
-      <c r="D12" s="2">
-        <f t="shared" ref="D12" si="1">A12*B12*C12</f>
+      <c r="D12" s="1">
+        <f t="shared" ref="D12:D13" si="2">A12*B12*C12</f>
         <v>1400000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>104000</v>
+      </c>
+      <c r="B13">
+        <v>14</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13" s="2">
+        <f t="shared" si="2"/>
+        <v>1456000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
everything prepared for c11 RNN run
</commit_message>
<xml_diff>
--- a/num_updats_calculations.xlsx
+++ b/num_updats_calculations.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="10">
   <si>
     <t>num_updates</t>
   </si>
@@ -51,6 +51,9 @@
   </si>
   <si>
     <t>number of years simulated</t>
+  </si>
+  <si>
+    <t>c7</t>
   </si>
 </sst>
 </file>
@@ -411,10 +414,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O13"/>
+  <dimension ref="A1:O14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -468,7 +471,7 @@
         <v>8</v>
       </c>
       <c r="D2" s="1">
-        <f t="shared" ref="D2:D11" si="0">A2*B2*C2</f>
+        <f t="shared" ref="D2:D12" si="0">A2*B2*C2</f>
         <v>1456000</v>
       </c>
       <c r="G2">
@@ -508,6 +511,9 @@
         <f t="shared" si="0"/>
         <v>2912000</v>
       </c>
+      <c r="E3" t="s">
+        <v>9</v>
+      </c>
       <c r="G3">
         <v>2912000</v>
       </c>
@@ -710,7 +716,7 @@
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>20000</v>
+        <v>2000</v>
       </c>
       <c r="B11">
         <v>14</v>
@@ -720,12 +726,12 @@
       </c>
       <c r="D11" s="1">
         <f t="shared" si="0"/>
-        <v>280000</v>
+        <v>28000</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>100000</v>
+        <v>20000</v>
       </c>
       <c r="B12">
         <v>14</v>
@@ -734,26 +740,42 @@
         <v>1</v>
       </c>
       <c r="D12" s="1">
-        <f t="shared" ref="D12:D13" si="2">A12*B12*C12</f>
-        <v>1400000</v>
+        <f t="shared" si="0"/>
+        <v>280000</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13">
+        <v>100000</v>
+      </c>
+      <c r="B13">
+        <v>14</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13" s="1">
+        <f t="shared" ref="D13:D14" si="2">A13*B13*C13</f>
+        <v>1400000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14">
         <v>104000</v>
       </c>
-      <c r="B13">
-        <v>14</v>
-      </c>
-      <c r="C13">
-        <v>1</v>
-      </c>
-      <c r="D13" s="2">
+      <c r="B14">
+        <v>14</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14" s="2">
         <f t="shared" si="2"/>
         <v>1456000</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
save current progress in feudal implementation. new feudalpolicy in model.py. not finished yet
</commit_message>
<xml_diff>
--- a/num_updats_calculations.xlsx
+++ b/num_updats_calculations.xlsx
@@ -414,10 +414,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O14"/>
+  <dimension ref="A1:O15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -535,7 +535,7 @@
         <v>26</v>
       </c>
       <c r="O3" s="1">
-        <f t="shared" ref="O3:O6" si="1">J3/M3</f>
+        <f t="shared" ref="O3:O7" si="1">J3/M3</f>
         <v>800</v>
       </c>
     </row>
@@ -666,6 +666,27 @@
         <f t="shared" si="0"/>
         <v>5824000</v>
       </c>
+      <c r="G7">
+        <v>2912000</v>
+      </c>
+      <c r="H7">
+        <v>14</v>
+      </c>
+      <c r="I7">
+        <v>14</v>
+      </c>
+      <c r="J7" s="2">
+        <f>G7/H7/I7</f>
+        <v>14857.142857142857</v>
+      </c>
+      <c r="M7" s="2">
+        <f>364/H7</f>
+        <v>26</v>
+      </c>
+      <c r="O7" s="2">
+        <f t="shared" si="1"/>
+        <v>571.42857142857144</v>
+      </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8">
@@ -755,7 +776,7 @@
         <v>1</v>
       </c>
       <c r="D13" s="1">
-        <f t="shared" ref="D13:D14" si="2">A13*B13*C13</f>
+        <f t="shared" ref="D13:D15" si="2">A13*B13*C13</f>
         <v>1400000</v>
       </c>
     </row>
@@ -772,6 +793,21 @@
       <c r="D14" s="2">
         <f t="shared" si="2"/>
         <v>1456000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>20000</v>
+      </c>
+      <c r="B15">
+        <v>14</v>
+      </c>
+      <c r="C15">
+        <v>14</v>
+      </c>
+      <c r="D15" s="2">
+        <f t="shared" si="2"/>
+        <v>3920000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>